<commit_message>
import / export using pandas
- changed import export to use the pandas library
- started to introduce a new class structure
</commit_message>
<xml_diff>
--- a/flicker.xlsx
+++ b/flicker.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\GitHub\bootstrapit\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\development\Github\bootstrapit\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11370"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11376"/>
   </bookViews>
   <sheets>
     <sheet name="flicker" sheetId="1" r:id="rId1"/>
@@ -515,48 +515,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -868,84 +868,96 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection sqref="A1:C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>26.8</v>
-      </c>
-      <c r="C1">
-        <v>27.9</v>
-      </c>
-      <c r="D1">
-        <v>23.7</v>
-      </c>
-      <c r="E1">
-        <v>25</v>
-      </c>
-      <c r="F1">
-        <v>26.3</v>
-      </c>
-      <c r="G1">
-        <v>24.8</v>
-      </c>
-      <c r="H1">
-        <v>25.7</v>
-      </c>
-      <c r="I1">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
       </c>
       <c r="B2">
         <v>26.4</v>
       </c>
       <c r="C2">
+        <v>25.7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>27.9</v>
+      </c>
+      <c r="B3">
         <v>24.2</v>
-      </c>
-      <c r="D2">
-        <v>28</v>
-      </c>
-      <c r="E2">
-        <v>26.9</v>
-      </c>
-      <c r="F2">
-        <v>29.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>25.7</v>
       </c>
       <c r="C3">
         <v>27.2</v>
       </c>
-      <c r="D3">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>23.7</v>
+      </c>
+      <c r="B4">
+        <v>28</v>
+      </c>
+      <c r="C4">
         <v>29.9</v>
       </c>
-      <c r="E3">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>26.9</v>
+      </c>
+      <c r="C5">
         <v>28.5</v>
       </c>
-      <c r="F3">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>26.3</v>
+      </c>
+      <c r="B6">
+        <v>29.1</v>
+      </c>
+      <c r="C6">
         <v>29.4</v>
       </c>
-      <c r="G3">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>24.8</v>
+      </c>
+      <c r="C7">
         <v>28.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>25.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>24.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>